<commit_message>
Added Shops excel file; rearranged menu items in index.html; replaced anchor tag with divs in services of landing_page
</commit_message>
<xml_diff>
--- a/expanded_shops.xlsx
+++ b/expanded_shops.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abann\OneDrive\Desktop\cash_crop_detection\PDD\PDD\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED1334E-8552-40DE-AA44-0B52BC654E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -163,8 +169,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,13 +233,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -271,7 +285,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -305,6 +319,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -339,9 +354,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -514,14 +530,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,7 +565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -555,13 +579,13 @@
         <v>36</v>
       </c>
       <c r="E2">
-        <v>27.71304</v>
+        <v>27.713039999999999</v>
       </c>
       <c r="F2">
-        <v>85.31798000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>85.317980000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -575,13 +599,13 @@
         <v>37</v>
       </c>
       <c r="E3">
-        <v>27.71704</v>
+        <v>27.717040000000001</v>
       </c>
       <c r="F3">
-        <v>85.30775</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>85.307749999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -595,13 +619,13 @@
         <v>38</v>
       </c>
       <c r="E4">
-        <v>27.6766</v>
+        <v>27.676600000000001</v>
       </c>
       <c r="F4">
         <v>85.3142</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -615,13 +639,13 @@
         <v>39</v>
       </c>
       <c r="E5">
-        <v>27.6667</v>
+        <v>27.666699999999999</v>
       </c>
       <c r="F5">
-        <v>85.3167</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>85.316699999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -635,13 +659,13 @@
         <v>40</v>
       </c>
       <c r="E6">
-        <v>28.2096</v>
+        <v>28.209599999999998</v>
       </c>
       <c r="F6">
-        <v>83.98560000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>83.985600000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -655,13 +679,13 @@
         <v>41</v>
       </c>
       <c r="E7">
-        <v>28.2097</v>
+        <v>28.209700000000002</v>
       </c>
       <c r="F7">
-        <v>83.986</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>83.986000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -675,13 +699,13 @@
         <v>42</v>
       </c>
       <c r="E8">
-        <v>26.4525</v>
+        <v>26.452500000000001</v>
       </c>
       <c r="F8">
-        <v>87.2718</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>87.271799999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -698,10 +722,10 @@
         <v>26.4526</v>
       </c>
       <c r="F9">
-        <v>87.2719</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>87.271900000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -721,7 +745,7 @@
         <v>83.45</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -735,13 +759,13 @@
         <v>45</v>
       </c>
       <c r="E11">
-        <v>27.7001</v>
+        <v>27.700099999999999</v>
       </c>
       <c r="F11">
-        <v>83.45010000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>83.450100000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -755,13 +779,13 @@
         <v>46</v>
       </c>
       <c r="E12">
-        <v>27.671</v>
+        <v>27.670999999999999</v>
       </c>
       <c r="F12">
-        <v>85.4278</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>85.427800000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -778,7 +802,7 @@
         <v>27.68</v>
       </c>
       <c r="F13">
-        <v>85.40000000000001</v>
+        <v>85.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>